<commit_message>
added a lot of new things
</commit_message>
<xml_diff>
--- a/Modulization.xlsx
+++ b/Modulization.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE72B7A6-B5BF-47A9-BF7B-24F87849D1CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
@@ -67,16 +66,46 @@
     <t>Nhận tín hiệu từ Firmware: không thể thối tiền vừa đưa vào không?</t>
   </si>
   <si>
-    <t>Nhận tín hiệu từ Firmware: tiín hiệu trạng thái giao hàng</t>
-  </si>
-  <si>
     <t>Nhận tín hiệu từ Firmware: thông báo nhận sản phẩm</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: tín hiệu trạng thái giao hàng</t>
+  </si>
+  <si>
+    <t>Truyền xuống Firmware: mua sản phẩm bằng tiền mặt</t>
+  </si>
+  <si>
+    <t>Truyền xuống Firmware: mua sản phẩm bằng Momo</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: nhận QR Code</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: Timeout Giao Dịch Momo</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware:Kết quả giao dịch Momo  (thành công/thất bại)</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: cập nhật tiền còn lại</t>
+  </si>
+  <si>
+    <t>Truyền xuống Firmware: Hủy giao dịch</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: Tổng tiền &gt; 50000</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: Máy không đủ tiền thối</t>
+  </si>
+  <si>
+    <t>Nhận tín hiệu từ Firmware: Không thể thối tiền vừa đưa vào</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +554,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -533,16 +562,130 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>